<commit_message>
sum 22 entered for nine
</commit_message>
<xml_diff>
--- a/data/SLMatchupsNine.xlsx
+++ b/data/SLMatchupsNine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B37A5C-13D6-4932-A2ED-CEABB473596B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8138C6-0C72-47BF-8270-4CC6444D7ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D330"/>
+  <dimension ref="A1:D679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
-      <selection activeCell="H332" sqref="H332"/>
+    <sheetView tabSelected="1" topLeftCell="A653" workbookViewId="0">
+      <selection activeCell="A680" sqref="A680"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4993,6 +4993,4892 @@
         <v>4</v>
       </c>
     </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>5</v>
+      </c>
+      <c r="B331">
+        <v>8</v>
+      </c>
+      <c r="C331">
+        <v>6</v>
+      </c>
+      <c r="D331">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>4</v>
+      </c>
+      <c r="B332">
+        <v>7</v>
+      </c>
+      <c r="C332">
+        <v>3</v>
+      </c>
+      <c r="D332">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>2</v>
+      </c>
+      <c r="B333">
+        <v>2</v>
+      </c>
+      <c r="C333">
+        <v>4</v>
+      </c>
+      <c r="D333">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>7</v>
+      </c>
+      <c r="B334">
+        <v>5</v>
+      </c>
+      <c r="C334">
+        <v>5</v>
+      </c>
+      <c r="D334">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>4</v>
+      </c>
+      <c r="B335">
+        <v>13</v>
+      </c>
+      <c r="C335">
+        <v>5</v>
+      </c>
+      <c r="D335">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>4</v>
+      </c>
+      <c r="B336">
+        <v>4</v>
+      </c>
+      <c r="C336">
+        <v>3</v>
+      </c>
+      <c r="D336">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>7</v>
+      </c>
+      <c r="B337">
+        <v>15</v>
+      </c>
+      <c r="C337">
+        <v>8</v>
+      </c>
+      <c r="D337">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>4</v>
+      </c>
+      <c r="B338">
+        <v>5</v>
+      </c>
+      <c r="C338">
+        <v>5</v>
+      </c>
+      <c r="D338">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>4</v>
+      </c>
+      <c r="B339">
+        <v>5</v>
+      </c>
+      <c r="C339">
+        <v>5</v>
+      </c>
+      <c r="D339">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>6</v>
+      </c>
+      <c r="B340">
+        <v>8</v>
+      </c>
+      <c r="C340">
+        <v>5</v>
+      </c>
+      <c r="D340">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>3</v>
+      </c>
+      <c r="B341">
+        <v>6</v>
+      </c>
+      <c r="C341">
+        <v>2</v>
+      </c>
+      <c r="D341">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>4</v>
+      </c>
+      <c r="B342">
+        <v>8</v>
+      </c>
+      <c r="C342">
+        <v>2</v>
+      </c>
+      <c r="D342">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>4</v>
+      </c>
+      <c r="B343">
+        <v>5</v>
+      </c>
+      <c r="C343">
+        <v>2</v>
+      </c>
+      <c r="D343">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>6</v>
+      </c>
+      <c r="B344">
+        <v>15</v>
+      </c>
+      <c r="C344">
+        <v>2</v>
+      </c>
+      <c r="D344">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>4</v>
+      </c>
+      <c r="B345">
+        <v>6</v>
+      </c>
+      <c r="C345">
+        <v>3</v>
+      </c>
+      <c r="D345">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>6</v>
+      </c>
+      <c r="B346">
+        <v>4</v>
+      </c>
+      <c r="C346">
+        <v>7</v>
+      </c>
+      <c r="D346">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>3</v>
+      </c>
+      <c r="B347">
+        <v>16</v>
+      </c>
+      <c r="C347">
+        <v>4</v>
+      </c>
+      <c r="D347">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>6</v>
+      </c>
+      <c r="B348">
+        <v>14</v>
+      </c>
+      <c r="C348">
+        <v>4</v>
+      </c>
+      <c r="D348">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>3</v>
+      </c>
+      <c r="B349">
+        <v>4</v>
+      </c>
+      <c r="C349">
+        <v>3</v>
+      </c>
+      <c r="D349">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>4</v>
+      </c>
+      <c r="B350">
+        <v>12</v>
+      </c>
+      <c r="C350">
+        <v>3</v>
+      </c>
+      <c r="D350">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>6</v>
+      </c>
+      <c r="B351">
+        <v>4</v>
+      </c>
+      <c r="C351">
+        <v>5</v>
+      </c>
+      <c r="D351">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>3</v>
+      </c>
+      <c r="B352">
+        <v>6</v>
+      </c>
+      <c r="C352">
+        <v>4</v>
+      </c>
+      <c r="D352">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>6</v>
+      </c>
+      <c r="B353">
+        <v>6</v>
+      </c>
+      <c r="C353">
+        <v>5</v>
+      </c>
+      <c r="D353">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>4</v>
+      </c>
+      <c r="B354">
+        <v>16</v>
+      </c>
+      <c r="C354">
+        <v>3</v>
+      </c>
+      <c r="D354">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>6</v>
+      </c>
+      <c r="B355">
+        <v>6</v>
+      </c>
+      <c r="C355">
+        <v>9</v>
+      </c>
+      <c r="D355">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>4</v>
+      </c>
+      <c r="B356">
+        <v>16</v>
+      </c>
+      <c r="C356">
+        <v>5</v>
+      </c>
+      <c r="D356">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>3</v>
+      </c>
+      <c r="B357">
+        <v>12</v>
+      </c>
+      <c r="C357">
+        <v>4</v>
+      </c>
+      <c r="D357">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>4</v>
+      </c>
+      <c r="B358">
+        <v>15</v>
+      </c>
+      <c r="C358">
+        <v>2</v>
+      </c>
+      <c r="D358">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>5</v>
+      </c>
+      <c r="B359">
+        <v>15</v>
+      </c>
+      <c r="C359">
+        <v>2</v>
+      </c>
+      <c r="D359">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>4</v>
+      </c>
+      <c r="B360">
+        <v>6</v>
+      </c>
+      <c r="C360">
+        <v>3</v>
+      </c>
+      <c r="D360">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>5</v>
+      </c>
+      <c r="B361">
+        <v>15</v>
+      </c>
+      <c r="C361">
+        <v>4</v>
+      </c>
+      <c r="D361">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>3</v>
+      </c>
+      <c r="B362">
+        <v>12</v>
+      </c>
+      <c r="C362">
+        <v>4</v>
+      </c>
+      <c r="D362">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>2</v>
+      </c>
+      <c r="B363">
+        <v>17</v>
+      </c>
+      <c r="C363">
+        <v>7</v>
+      </c>
+      <c r="D363">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>5</v>
+      </c>
+      <c r="B364">
+        <v>8</v>
+      </c>
+      <c r="C364">
+        <v>4</v>
+      </c>
+      <c r="D364">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>5</v>
+      </c>
+      <c r="B365">
+        <v>7</v>
+      </c>
+      <c r="C365">
+        <v>4</v>
+      </c>
+      <c r="D365">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>3</v>
+      </c>
+      <c r="B366">
+        <v>12</v>
+      </c>
+      <c r="C366">
+        <v>4</v>
+      </c>
+      <c r="D366">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>2</v>
+      </c>
+      <c r="B367">
+        <v>2</v>
+      </c>
+      <c r="C367">
+        <v>5</v>
+      </c>
+      <c r="D367">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>7</v>
+      </c>
+      <c r="B368">
+        <v>6</v>
+      </c>
+      <c r="C368">
+        <v>6</v>
+      </c>
+      <c r="D368">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>7</v>
+      </c>
+      <c r="B369">
+        <v>1</v>
+      </c>
+      <c r="C369">
+        <v>2</v>
+      </c>
+      <c r="D369">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>4</v>
+      </c>
+      <c r="B370">
+        <v>8</v>
+      </c>
+      <c r="C370">
+        <v>6</v>
+      </c>
+      <c r="D370">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>6</v>
+      </c>
+      <c r="B371">
+        <v>14</v>
+      </c>
+      <c r="C371">
+        <v>7</v>
+      </c>
+      <c r="D371">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>3</v>
+      </c>
+      <c r="B372">
+        <v>4</v>
+      </c>
+      <c r="C372">
+        <v>4</v>
+      </c>
+      <c r="D372">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>5</v>
+      </c>
+      <c r="B373">
+        <v>6</v>
+      </c>
+      <c r="C373">
+        <v>3</v>
+      </c>
+      <c r="D373">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>4</v>
+      </c>
+      <c r="B374">
+        <v>4</v>
+      </c>
+      <c r="C374">
+        <v>2</v>
+      </c>
+      <c r="D374">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>3</v>
+      </c>
+      <c r="B375">
+        <v>15</v>
+      </c>
+      <c r="C375">
+        <v>2</v>
+      </c>
+      <c r="D375">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>4</v>
+      </c>
+      <c r="B376">
+        <v>14</v>
+      </c>
+      <c r="C376">
+        <v>3</v>
+      </c>
+      <c r="D376">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>4</v>
+      </c>
+      <c r="B377">
+        <v>6</v>
+      </c>
+      <c r="C377">
+        <v>6</v>
+      </c>
+      <c r="D377">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>5</v>
+      </c>
+      <c r="B378">
+        <v>4</v>
+      </c>
+      <c r="C378">
+        <v>6</v>
+      </c>
+      <c r="D378">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>5</v>
+      </c>
+      <c r="B379">
+        <v>8</v>
+      </c>
+      <c r="C379">
+        <v>4</v>
+      </c>
+      <c r="D379">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>5</v>
+      </c>
+      <c r="B380">
+        <v>13</v>
+      </c>
+      <c r="C380">
+        <v>3</v>
+      </c>
+      <c r="D380">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>2</v>
+      </c>
+      <c r="B381">
+        <v>4</v>
+      </c>
+      <c r="C381">
+        <v>1</v>
+      </c>
+      <c r="D381">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>5</v>
+      </c>
+      <c r="B382">
+        <v>18</v>
+      </c>
+      <c r="C382">
+        <v>4</v>
+      </c>
+      <c r="D382">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>7</v>
+      </c>
+      <c r="B383">
+        <v>14</v>
+      </c>
+      <c r="C383">
+        <v>5</v>
+      </c>
+      <c r="D383">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>3</v>
+      </c>
+      <c r="B384">
+        <v>14</v>
+      </c>
+      <c r="C384">
+        <v>2</v>
+      </c>
+      <c r="D384">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>4</v>
+      </c>
+      <c r="B385">
+        <v>8</v>
+      </c>
+      <c r="C385">
+        <v>6</v>
+      </c>
+      <c r="D385">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>4</v>
+      </c>
+      <c r="B386">
+        <v>4</v>
+      </c>
+      <c r="C386">
+        <v>2</v>
+      </c>
+      <c r="D386">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>4</v>
+      </c>
+      <c r="B387">
+        <v>16</v>
+      </c>
+      <c r="C387">
+        <v>3</v>
+      </c>
+      <c r="D387">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>4</v>
+      </c>
+      <c r="B388">
+        <v>6</v>
+      </c>
+      <c r="C388">
+        <v>2</v>
+      </c>
+      <c r="D388">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>6</v>
+      </c>
+      <c r="B389">
+        <v>12</v>
+      </c>
+      <c r="C389">
+        <v>7</v>
+      </c>
+      <c r="D389">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>4</v>
+      </c>
+      <c r="B390">
+        <v>6</v>
+      </c>
+      <c r="C390">
+        <v>3</v>
+      </c>
+      <c r="D390">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>5</v>
+      </c>
+      <c r="B391">
+        <v>13</v>
+      </c>
+      <c r="C391">
+        <v>4</v>
+      </c>
+      <c r="D391">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>3</v>
+      </c>
+      <c r="B392">
+        <v>8</v>
+      </c>
+      <c r="C392">
+        <v>5</v>
+      </c>
+      <c r="D392">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>4</v>
+      </c>
+      <c r="B393">
+        <v>15</v>
+      </c>
+      <c r="C393">
+        <v>6</v>
+      </c>
+      <c r="D393">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>4</v>
+      </c>
+      <c r="B394">
+        <v>4</v>
+      </c>
+      <c r="C394">
+        <v>5</v>
+      </c>
+      <c r="D394">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>6</v>
+      </c>
+      <c r="B395">
+        <v>8</v>
+      </c>
+      <c r="C395">
+        <v>5</v>
+      </c>
+      <c r="D395">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>2</v>
+      </c>
+      <c r="B396">
+        <v>6</v>
+      </c>
+      <c r="C396">
+        <v>4</v>
+      </c>
+      <c r="D396">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>4</v>
+      </c>
+      <c r="B397">
+        <v>6</v>
+      </c>
+      <c r="C397">
+        <v>5</v>
+      </c>
+      <c r="D397">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>4</v>
+      </c>
+      <c r="B398">
+        <v>7</v>
+      </c>
+      <c r="C398">
+        <v>1</v>
+      </c>
+      <c r="D398">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>4</v>
+      </c>
+      <c r="B399">
+        <v>12</v>
+      </c>
+      <c r="C399">
+        <v>5</v>
+      </c>
+      <c r="D399">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>3</v>
+      </c>
+      <c r="B400">
+        <v>14</v>
+      </c>
+      <c r="C400">
+        <v>2</v>
+      </c>
+      <c r="D400">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>2</v>
+      </c>
+      <c r="B401">
+        <v>13</v>
+      </c>
+      <c r="C401">
+        <v>3</v>
+      </c>
+      <c r="D401">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>2</v>
+      </c>
+      <c r="B402">
+        <v>4</v>
+      </c>
+      <c r="C402">
+        <v>3</v>
+      </c>
+      <c r="D402">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>2</v>
+      </c>
+      <c r="B403">
+        <v>6</v>
+      </c>
+      <c r="C403">
+        <v>7</v>
+      </c>
+      <c r="D403">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>2</v>
+      </c>
+      <c r="B404">
+        <v>8</v>
+      </c>
+      <c r="C404">
+        <v>4</v>
+      </c>
+      <c r="D404">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>6</v>
+      </c>
+      <c r="B405">
+        <v>16</v>
+      </c>
+      <c r="C405">
+        <v>4</v>
+      </c>
+      <c r="D405">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>3</v>
+      </c>
+      <c r="B406">
+        <v>14</v>
+      </c>
+      <c r="C406">
+        <v>4</v>
+      </c>
+      <c r="D406">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>5</v>
+      </c>
+      <c r="B407">
+        <v>12</v>
+      </c>
+      <c r="C407">
+        <v>6</v>
+      </c>
+      <c r="D407">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>5</v>
+      </c>
+      <c r="B408">
+        <v>7</v>
+      </c>
+      <c r="C408">
+        <v>6</v>
+      </c>
+      <c r="D408">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>5</v>
+      </c>
+      <c r="B409">
+        <v>6</v>
+      </c>
+      <c r="C409">
+        <v>2</v>
+      </c>
+      <c r="D409">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>2</v>
+      </c>
+      <c r="B410">
+        <v>7</v>
+      </c>
+      <c r="C410">
+        <v>6</v>
+      </c>
+      <c r="D410">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>3</v>
+      </c>
+      <c r="B411">
+        <v>16</v>
+      </c>
+      <c r="C411">
+        <v>2</v>
+      </c>
+      <c r="D411">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>5</v>
+      </c>
+      <c r="B412">
+        <v>2</v>
+      </c>
+      <c r="C412">
+        <v>3</v>
+      </c>
+      <c r="D412">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>2</v>
+      </c>
+      <c r="B413">
+        <v>16</v>
+      </c>
+      <c r="C413">
+        <v>3</v>
+      </c>
+      <c r="D413">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>5</v>
+      </c>
+      <c r="B414">
+        <v>6</v>
+      </c>
+      <c r="C414">
+        <v>4</v>
+      </c>
+      <c r="D414">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>5</v>
+      </c>
+      <c r="B415">
+        <v>16</v>
+      </c>
+      <c r="C415">
+        <v>6</v>
+      </c>
+      <c r="D415">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>1</v>
+      </c>
+      <c r="B416">
+        <v>6</v>
+      </c>
+      <c r="C416">
+        <v>4</v>
+      </c>
+      <c r="D416">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>9</v>
+      </c>
+      <c r="B417">
+        <v>7</v>
+      </c>
+      <c r="C417">
+        <v>7</v>
+      </c>
+      <c r="D417">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>5</v>
+      </c>
+      <c r="B418">
+        <v>12</v>
+      </c>
+      <c r="C418">
+        <v>4</v>
+      </c>
+      <c r="D418">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>3</v>
+      </c>
+      <c r="B419">
+        <v>8</v>
+      </c>
+      <c r="C419">
+        <v>4</v>
+      </c>
+      <c r="D419">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>3</v>
+      </c>
+      <c r="B420">
+        <v>6</v>
+      </c>
+      <c r="C420">
+        <v>2</v>
+      </c>
+      <c r="D420">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>4</v>
+      </c>
+      <c r="B421">
+        <v>15</v>
+      </c>
+      <c r="C421">
+        <v>3</v>
+      </c>
+      <c r="D421">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>4</v>
+      </c>
+      <c r="B422">
+        <v>13</v>
+      </c>
+      <c r="C422">
+        <v>5</v>
+      </c>
+      <c r="D422">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>4</v>
+      </c>
+      <c r="B423">
+        <v>1</v>
+      </c>
+      <c r="C423">
+        <v>5</v>
+      </c>
+      <c r="D423">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>6</v>
+      </c>
+      <c r="B424">
+        <v>12</v>
+      </c>
+      <c r="C424">
+        <v>4</v>
+      </c>
+      <c r="D424">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>6</v>
+      </c>
+      <c r="B425">
+        <v>15</v>
+      </c>
+      <c r="C425">
+        <v>2</v>
+      </c>
+      <c r="D425">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>7</v>
+      </c>
+      <c r="B426">
+        <v>7</v>
+      </c>
+      <c r="C426">
+        <v>4</v>
+      </c>
+      <c r="D426">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>4</v>
+      </c>
+      <c r="B427">
+        <v>6</v>
+      </c>
+      <c r="C427">
+        <v>8</v>
+      </c>
+      <c r="D427">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>6</v>
+      </c>
+      <c r="B428">
+        <v>12</v>
+      </c>
+      <c r="C428">
+        <v>5</v>
+      </c>
+      <c r="D428">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>6</v>
+      </c>
+      <c r="B429">
+        <v>18</v>
+      </c>
+      <c r="C429">
+        <v>3</v>
+      </c>
+      <c r="D429">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>2</v>
+      </c>
+      <c r="B430">
+        <v>2</v>
+      </c>
+      <c r="C430">
+        <v>5</v>
+      </c>
+      <c r="D430">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>2</v>
+      </c>
+      <c r="B431">
+        <v>17</v>
+      </c>
+      <c r="C431">
+        <v>4</v>
+      </c>
+      <c r="D431">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>4</v>
+      </c>
+      <c r="B432">
+        <v>8</v>
+      </c>
+      <c r="C432">
+        <v>6</v>
+      </c>
+      <c r="D432">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>4</v>
+      </c>
+      <c r="B433">
+        <v>7</v>
+      </c>
+      <c r="C433">
+        <v>7</v>
+      </c>
+      <c r="D433">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>3</v>
+      </c>
+      <c r="B434">
+        <v>12</v>
+      </c>
+      <c r="C434">
+        <v>2</v>
+      </c>
+      <c r="D434">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>4</v>
+      </c>
+      <c r="B435">
+        <v>13</v>
+      </c>
+      <c r="C435">
+        <v>5</v>
+      </c>
+      <c r="D435">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>4</v>
+      </c>
+      <c r="B436">
+        <v>5</v>
+      </c>
+      <c r="C436">
+        <v>2</v>
+      </c>
+      <c r="D436">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>3</v>
+      </c>
+      <c r="B437">
+        <v>18</v>
+      </c>
+      <c r="C437">
+        <v>4</v>
+      </c>
+      <c r="D437">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>4</v>
+      </c>
+      <c r="B438">
+        <v>8</v>
+      </c>
+      <c r="C438">
+        <v>3</v>
+      </c>
+      <c r="D438">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>3</v>
+      </c>
+      <c r="B439">
+        <v>16</v>
+      </c>
+      <c r="C439">
+        <v>2</v>
+      </c>
+      <c r="D439">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>4</v>
+      </c>
+      <c r="B440">
+        <v>5</v>
+      </c>
+      <c r="C440">
+        <v>7</v>
+      </c>
+      <c r="D440">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>5</v>
+      </c>
+      <c r="B441">
+        <v>6</v>
+      </c>
+      <c r="C441">
+        <v>4</v>
+      </c>
+      <c r="D441">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>3</v>
+      </c>
+      <c r="B442">
+        <v>8</v>
+      </c>
+      <c r="C442">
+        <v>4</v>
+      </c>
+      <c r="D442">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>3</v>
+      </c>
+      <c r="B443">
+        <v>13</v>
+      </c>
+      <c r="C443">
+        <v>4</v>
+      </c>
+      <c r="D443">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>5</v>
+      </c>
+      <c r="B444">
+        <v>14</v>
+      </c>
+      <c r="C444">
+        <v>4</v>
+      </c>
+      <c r="D444">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>2</v>
+      </c>
+      <c r="B445">
+        <v>13</v>
+      </c>
+      <c r="C445">
+        <v>4</v>
+      </c>
+      <c r="D445">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>3</v>
+      </c>
+      <c r="B446">
+        <v>17</v>
+      </c>
+      <c r="C446">
+        <v>4</v>
+      </c>
+      <c r="D446">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>2</v>
+      </c>
+      <c r="B447">
+        <v>5</v>
+      </c>
+      <c r="C447">
+        <v>4</v>
+      </c>
+      <c r="D447">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>5</v>
+      </c>
+      <c r="B448">
+        <v>13</v>
+      </c>
+      <c r="C448">
+        <v>6</v>
+      </c>
+      <c r="D448">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>2</v>
+      </c>
+      <c r="B449">
+        <v>6</v>
+      </c>
+      <c r="C449">
+        <v>4</v>
+      </c>
+      <c r="D449">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>5</v>
+      </c>
+      <c r="B450">
+        <v>16</v>
+      </c>
+      <c r="C450">
+        <v>6</v>
+      </c>
+      <c r="D450">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>5</v>
+      </c>
+      <c r="B451">
+        <v>14</v>
+      </c>
+      <c r="C451">
+        <v>6</v>
+      </c>
+      <c r="D451">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>7</v>
+      </c>
+      <c r="B452">
+        <v>7</v>
+      </c>
+      <c r="C452">
+        <v>4</v>
+      </c>
+      <c r="D452">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>7</v>
+      </c>
+      <c r="B453">
+        <v>13</v>
+      </c>
+      <c r="C453">
+        <v>6</v>
+      </c>
+      <c r="D453">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>6</v>
+      </c>
+      <c r="B454">
+        <v>3</v>
+      </c>
+      <c r="C454">
+        <v>4</v>
+      </c>
+      <c r="D454">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>1</v>
+      </c>
+      <c r="B455">
+        <v>13</v>
+      </c>
+      <c r="C455">
+        <v>3</v>
+      </c>
+      <c r="D455">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>8</v>
+      </c>
+      <c r="B456">
+        <v>8</v>
+      </c>
+      <c r="C456">
+        <v>7</v>
+      </c>
+      <c r="D456">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>3</v>
+      </c>
+      <c r="B457">
+        <v>7</v>
+      </c>
+      <c r="C457">
+        <v>4</v>
+      </c>
+      <c r="D457">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>3</v>
+      </c>
+      <c r="B458">
+        <v>8</v>
+      </c>
+      <c r="C458">
+        <v>4</v>
+      </c>
+      <c r="D458">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>2</v>
+      </c>
+      <c r="B459">
+        <v>12</v>
+      </c>
+      <c r="C459">
+        <v>3</v>
+      </c>
+      <c r="D459">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>6</v>
+      </c>
+      <c r="B460">
+        <v>12</v>
+      </c>
+      <c r="C460">
+        <v>4</v>
+      </c>
+      <c r="D460">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>5</v>
+      </c>
+      <c r="B461">
+        <v>13</v>
+      </c>
+      <c r="C461">
+        <v>4</v>
+      </c>
+      <c r="D461">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>4</v>
+      </c>
+      <c r="B462">
+        <v>16</v>
+      </c>
+      <c r="C462">
+        <v>3</v>
+      </c>
+      <c r="D462">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>1</v>
+      </c>
+      <c r="B463">
+        <v>8</v>
+      </c>
+      <c r="C463">
+        <v>4</v>
+      </c>
+      <c r="D463">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>6</v>
+      </c>
+      <c r="B464">
+        <v>6</v>
+      </c>
+      <c r="C464">
+        <v>3</v>
+      </c>
+      <c r="D464">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>2</v>
+      </c>
+      <c r="B465">
+        <v>15</v>
+      </c>
+      <c r="C465">
+        <v>4</v>
+      </c>
+      <c r="D465">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>4</v>
+      </c>
+      <c r="B466">
+        <v>4</v>
+      </c>
+      <c r="C466">
+        <v>1</v>
+      </c>
+      <c r="D466">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>6</v>
+      </c>
+      <c r="B467">
+        <v>14</v>
+      </c>
+      <c r="C467">
+        <v>4</v>
+      </c>
+      <c r="D467">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>3</v>
+      </c>
+      <c r="B468">
+        <v>13</v>
+      </c>
+      <c r="C468">
+        <v>4</v>
+      </c>
+      <c r="D468">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A469">
+        <v>5</v>
+      </c>
+      <c r="B469">
+        <v>5</v>
+      </c>
+      <c r="C469">
+        <v>6</v>
+      </c>
+      <c r="D469">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A470">
+        <v>6</v>
+      </c>
+      <c r="B470">
+        <v>5</v>
+      </c>
+      <c r="C470">
+        <v>4</v>
+      </c>
+      <c r="D470">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471">
+        <v>5</v>
+      </c>
+      <c r="B471">
+        <v>16</v>
+      </c>
+      <c r="C471">
+        <v>4</v>
+      </c>
+      <c r="D471">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A472">
+        <v>2</v>
+      </c>
+      <c r="B472">
+        <v>6</v>
+      </c>
+      <c r="C472">
+        <v>1</v>
+      </c>
+      <c r="D472">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A473">
+        <v>7</v>
+      </c>
+      <c r="B473">
+        <v>3</v>
+      </c>
+      <c r="C473">
+        <v>5</v>
+      </c>
+      <c r="D473">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>3</v>
+      </c>
+      <c r="B474">
+        <v>6</v>
+      </c>
+      <c r="C474">
+        <v>5</v>
+      </c>
+      <c r="D474">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>4</v>
+      </c>
+      <c r="B475">
+        <v>14</v>
+      </c>
+      <c r="C475">
+        <v>3</v>
+      </c>
+      <c r="D475">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A476">
+        <v>3</v>
+      </c>
+      <c r="B476">
+        <v>3</v>
+      </c>
+      <c r="C476">
+        <v>2</v>
+      </c>
+      <c r="D476">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A477">
+        <v>5</v>
+      </c>
+      <c r="B477">
+        <v>17</v>
+      </c>
+      <c r="C477">
+        <v>1</v>
+      </c>
+      <c r="D477">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A478">
+        <v>5</v>
+      </c>
+      <c r="B478">
+        <v>7</v>
+      </c>
+      <c r="C478">
+        <v>6</v>
+      </c>
+      <c r="D478">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A479">
+        <v>5</v>
+      </c>
+      <c r="B479">
+        <v>14</v>
+      </c>
+      <c r="C479">
+        <v>7</v>
+      </c>
+      <c r="D479">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A480">
+        <v>2</v>
+      </c>
+      <c r="B480">
+        <v>12</v>
+      </c>
+      <c r="C480">
+        <v>1</v>
+      </c>
+      <c r="D480">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A481">
+        <v>9</v>
+      </c>
+      <c r="B481">
+        <v>13</v>
+      </c>
+      <c r="C481">
+        <v>4</v>
+      </c>
+      <c r="D481">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A482">
+        <v>2</v>
+      </c>
+      <c r="B482">
+        <v>6</v>
+      </c>
+      <c r="C482">
+        <v>4</v>
+      </c>
+      <c r="D482">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A483">
+        <v>3</v>
+      </c>
+      <c r="B483">
+        <v>8</v>
+      </c>
+      <c r="C483">
+        <v>4</v>
+      </c>
+      <c r="D483">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A484">
+        <v>4</v>
+      </c>
+      <c r="B484">
+        <v>12</v>
+      </c>
+      <c r="C484">
+        <v>3</v>
+      </c>
+      <c r="D484">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A485">
+        <v>1</v>
+      </c>
+      <c r="B485">
+        <v>18</v>
+      </c>
+      <c r="C485">
+        <v>3</v>
+      </c>
+      <c r="D485">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A486">
+        <v>1</v>
+      </c>
+      <c r="B486">
+        <v>14</v>
+      </c>
+      <c r="C486">
+        <v>3</v>
+      </c>
+      <c r="D486">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A487">
+        <v>5</v>
+      </c>
+      <c r="B487">
+        <v>7</v>
+      </c>
+      <c r="C487">
+        <v>6</v>
+      </c>
+      <c r="D487">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A488">
+        <v>7</v>
+      </c>
+      <c r="B488">
+        <v>15</v>
+      </c>
+      <c r="C488">
+        <v>5</v>
+      </c>
+      <c r="D488">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A489">
+        <v>5</v>
+      </c>
+      <c r="B489">
+        <v>6</v>
+      </c>
+      <c r="C489">
+        <v>4</v>
+      </c>
+      <c r="D489">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A490">
+        <v>3</v>
+      </c>
+      <c r="B490">
+        <v>13</v>
+      </c>
+      <c r="C490">
+        <v>4</v>
+      </c>
+      <c r="D490">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A491">
+        <v>6</v>
+      </c>
+      <c r="B491">
+        <v>15</v>
+      </c>
+      <c r="C491">
+        <v>5</v>
+      </c>
+      <c r="D491">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A492">
+        <v>5</v>
+      </c>
+      <c r="B492">
+        <v>19</v>
+      </c>
+      <c r="C492">
+        <v>3</v>
+      </c>
+      <c r="D492">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A493">
+        <v>3</v>
+      </c>
+      <c r="B493">
+        <v>8</v>
+      </c>
+      <c r="C493">
+        <v>4</v>
+      </c>
+      <c r="D493">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A494">
+        <v>4</v>
+      </c>
+      <c r="B494">
+        <v>14</v>
+      </c>
+      <c r="C494">
+        <v>5</v>
+      </c>
+      <c r="D494">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A495">
+        <v>5</v>
+      </c>
+      <c r="B495">
+        <v>5</v>
+      </c>
+      <c r="C495">
+        <v>6</v>
+      </c>
+      <c r="D495">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A496">
+        <v>5</v>
+      </c>
+      <c r="B496">
+        <v>5</v>
+      </c>
+      <c r="C496">
+        <v>4</v>
+      </c>
+      <c r="D496">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A497">
+        <v>2</v>
+      </c>
+      <c r="B497">
+        <v>8</v>
+      </c>
+      <c r="C497">
+        <v>4</v>
+      </c>
+      <c r="D497">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A498">
+        <v>4</v>
+      </c>
+      <c r="B498">
+        <v>12</v>
+      </c>
+      <c r="C498">
+        <v>5</v>
+      </c>
+      <c r="D498">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A499">
+        <v>3</v>
+      </c>
+      <c r="B499">
+        <v>15</v>
+      </c>
+      <c r="C499">
+        <v>2</v>
+      </c>
+      <c r="D499">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A500">
+        <v>4</v>
+      </c>
+      <c r="B500">
+        <v>6</v>
+      </c>
+      <c r="C500">
+        <v>3</v>
+      </c>
+      <c r="D500">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A501">
+        <v>6</v>
+      </c>
+      <c r="B501">
+        <v>8</v>
+      </c>
+      <c r="C501">
+        <v>5</v>
+      </c>
+      <c r="D501">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A502">
+        <v>4</v>
+      </c>
+      <c r="B502">
+        <v>8</v>
+      </c>
+      <c r="C502">
+        <v>8</v>
+      </c>
+      <c r="D502">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A503">
+        <v>4</v>
+      </c>
+      <c r="B503">
+        <v>3</v>
+      </c>
+      <c r="C503">
+        <v>1</v>
+      </c>
+      <c r="D503">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A504">
+        <v>4</v>
+      </c>
+      <c r="B504">
+        <v>12</v>
+      </c>
+      <c r="C504">
+        <v>6</v>
+      </c>
+      <c r="D504">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A505">
+        <v>3</v>
+      </c>
+      <c r="B505">
+        <v>2</v>
+      </c>
+      <c r="C505">
+        <v>2</v>
+      </c>
+      <c r="D505">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A506">
+        <v>4</v>
+      </c>
+      <c r="B506">
+        <v>13</v>
+      </c>
+      <c r="C506">
+        <v>6</v>
+      </c>
+      <c r="D506">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A507">
+        <v>4</v>
+      </c>
+      <c r="B507">
+        <v>3</v>
+      </c>
+      <c r="C507">
+        <v>2</v>
+      </c>
+      <c r="D507">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A508">
+        <v>7</v>
+      </c>
+      <c r="B508">
+        <v>14</v>
+      </c>
+      <c r="C508">
+        <v>6</v>
+      </c>
+      <c r="D508">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A509">
+        <v>4</v>
+      </c>
+      <c r="B509">
+        <v>12</v>
+      </c>
+      <c r="C509">
+        <v>3</v>
+      </c>
+      <c r="D509">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A510">
+        <v>1</v>
+      </c>
+      <c r="B510">
+        <v>1</v>
+      </c>
+      <c r="C510">
+        <v>4</v>
+      </c>
+      <c r="D510">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A511">
+        <v>6</v>
+      </c>
+      <c r="B511">
+        <v>5</v>
+      </c>
+      <c r="C511">
+        <v>5</v>
+      </c>
+      <c r="D511">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A512">
+        <v>3</v>
+      </c>
+      <c r="B512">
+        <v>14</v>
+      </c>
+      <c r="C512">
+        <v>1</v>
+      </c>
+      <c r="D512">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A513">
+        <v>6</v>
+      </c>
+      <c r="B513">
+        <v>8</v>
+      </c>
+      <c r="C513">
+        <v>4</v>
+      </c>
+      <c r="D513">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A514">
+        <v>2</v>
+      </c>
+      <c r="B514">
+        <v>16</v>
+      </c>
+      <c r="C514">
+        <v>4</v>
+      </c>
+      <c r="D514">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A515">
+        <v>4</v>
+      </c>
+      <c r="B515">
+        <v>6</v>
+      </c>
+      <c r="C515">
+        <v>5</v>
+      </c>
+      <c r="D515">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A516">
+        <v>1</v>
+      </c>
+      <c r="B516">
+        <v>14</v>
+      </c>
+      <c r="C516">
+        <v>3</v>
+      </c>
+      <c r="D516">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A517">
+        <v>7</v>
+      </c>
+      <c r="B517">
+        <v>16</v>
+      </c>
+      <c r="C517">
+        <v>6</v>
+      </c>
+      <c r="D517">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A518">
+        <v>3</v>
+      </c>
+      <c r="B518">
+        <v>1</v>
+      </c>
+      <c r="C518">
+        <v>2</v>
+      </c>
+      <c r="D518">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A519">
+        <v>3</v>
+      </c>
+      <c r="B519">
+        <v>6</v>
+      </c>
+      <c r="C519">
+        <v>2</v>
+      </c>
+      <c r="D519">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A520">
+        <v>6</v>
+      </c>
+      <c r="B520">
+        <v>8</v>
+      </c>
+      <c r="C520">
+        <v>5</v>
+      </c>
+      <c r="D520">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A521">
+        <v>4</v>
+      </c>
+      <c r="B521">
+        <v>12</v>
+      </c>
+      <c r="C521">
+        <v>3</v>
+      </c>
+      <c r="D521">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="522" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A522">
+        <v>6</v>
+      </c>
+      <c r="B522">
+        <v>6</v>
+      </c>
+      <c r="C522">
+        <v>9</v>
+      </c>
+      <c r="D522">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A523">
+        <v>2</v>
+      </c>
+      <c r="B523">
+        <v>4</v>
+      </c>
+      <c r="C523">
+        <v>3</v>
+      </c>
+      <c r="D523">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="524" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A524">
+        <v>6</v>
+      </c>
+      <c r="B524">
+        <v>12</v>
+      </c>
+      <c r="C524">
+        <v>4</v>
+      </c>
+      <c r="D524">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="525" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A525">
+        <v>2</v>
+      </c>
+      <c r="B525">
+        <v>7</v>
+      </c>
+      <c r="C525">
+        <v>4</v>
+      </c>
+      <c r="D525">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="526" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A526">
+        <v>6</v>
+      </c>
+      <c r="B526">
+        <v>12</v>
+      </c>
+      <c r="C526">
+        <v>4</v>
+      </c>
+      <c r="D526">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="527" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A527">
+        <v>1</v>
+      </c>
+      <c r="B527">
+        <v>14</v>
+      </c>
+      <c r="C527">
+        <v>3</v>
+      </c>
+      <c r="D527">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="528" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A528">
+        <v>5</v>
+      </c>
+      <c r="B528">
+        <v>12</v>
+      </c>
+      <c r="C528">
+        <v>4</v>
+      </c>
+      <c r="D528">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="529" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A529">
+        <v>5</v>
+      </c>
+      <c r="B529">
+        <v>14</v>
+      </c>
+      <c r="C529">
+        <v>4</v>
+      </c>
+      <c r="D529">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A530">
+        <v>3</v>
+      </c>
+      <c r="B530">
+        <v>7</v>
+      </c>
+      <c r="C530">
+        <v>4</v>
+      </c>
+      <c r="D530">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="531" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A531">
+        <v>4</v>
+      </c>
+      <c r="B531">
+        <v>8</v>
+      </c>
+      <c r="C531">
+        <v>3</v>
+      </c>
+      <c r="D531">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A532">
+        <v>4</v>
+      </c>
+      <c r="B532">
+        <v>8</v>
+      </c>
+      <c r="C532">
+        <v>1</v>
+      </c>
+      <c r="D532">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A533">
+        <v>4</v>
+      </c>
+      <c r="B533">
+        <v>18</v>
+      </c>
+      <c r="C533">
+        <v>4</v>
+      </c>
+      <c r="D533">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A534">
+        <v>3</v>
+      </c>
+      <c r="B534">
+        <v>7</v>
+      </c>
+      <c r="C534">
+        <v>4</v>
+      </c>
+      <c r="D534">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A535">
+        <v>4</v>
+      </c>
+      <c r="B535">
+        <v>2</v>
+      </c>
+      <c r="C535">
+        <v>2</v>
+      </c>
+      <c r="D535">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A536">
+        <v>4</v>
+      </c>
+      <c r="B536">
+        <v>6</v>
+      </c>
+      <c r="C536">
+        <v>5</v>
+      </c>
+      <c r="D536">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A537">
+        <v>3</v>
+      </c>
+      <c r="B537">
+        <v>13</v>
+      </c>
+      <c r="C537">
+        <v>5</v>
+      </c>
+      <c r="D537">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A538">
+        <v>5</v>
+      </c>
+      <c r="B538">
+        <v>8</v>
+      </c>
+      <c r="C538">
+        <v>7</v>
+      </c>
+      <c r="D538">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A539">
+        <v>6</v>
+      </c>
+      <c r="B539">
+        <v>2</v>
+      </c>
+      <c r="C539">
+        <v>2</v>
+      </c>
+      <c r="D539">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A540">
+        <v>3</v>
+      </c>
+      <c r="B540">
+        <v>5</v>
+      </c>
+      <c r="C540">
+        <v>5</v>
+      </c>
+      <c r="D540">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A541">
+        <v>2</v>
+      </c>
+      <c r="B541">
+        <v>13</v>
+      </c>
+      <c r="C541">
+        <v>3</v>
+      </c>
+      <c r="D541">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A542">
+        <v>5</v>
+      </c>
+      <c r="B542">
+        <v>12</v>
+      </c>
+      <c r="C542">
+        <v>6</v>
+      </c>
+      <c r="D542">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A543">
+        <v>4</v>
+      </c>
+      <c r="B543">
+        <v>12</v>
+      </c>
+      <c r="C543">
+        <v>5</v>
+      </c>
+      <c r="D543">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A544">
+        <v>5</v>
+      </c>
+      <c r="B544">
+        <v>15</v>
+      </c>
+      <c r="C544">
+        <v>6</v>
+      </c>
+      <c r="D544">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A545">
+        <v>3</v>
+      </c>
+      <c r="B545">
+        <v>16</v>
+      </c>
+      <c r="C545">
+        <v>4</v>
+      </c>
+      <c r="D545">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="546" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A546">
+        <v>2</v>
+      </c>
+      <c r="B546">
+        <v>8</v>
+      </c>
+      <c r="C546">
+        <v>3</v>
+      </c>
+      <c r="D546">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A547">
+        <v>9</v>
+      </c>
+      <c r="B547">
+        <v>7</v>
+      </c>
+      <c r="C547">
+        <v>6</v>
+      </c>
+      <c r="D547">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A548">
+        <v>4</v>
+      </c>
+      <c r="B548">
+        <v>13</v>
+      </c>
+      <c r="C548">
+        <v>6</v>
+      </c>
+      <c r="D548">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A549">
+        <v>4</v>
+      </c>
+      <c r="B549">
+        <v>14</v>
+      </c>
+      <c r="C549">
+        <v>3</v>
+      </c>
+      <c r="D549">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A550">
+        <v>4</v>
+      </c>
+      <c r="B550">
+        <v>5</v>
+      </c>
+      <c r="C550">
+        <v>6</v>
+      </c>
+      <c r="D550">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A551">
+        <v>7</v>
+      </c>
+      <c r="B551">
+        <v>5</v>
+      </c>
+      <c r="C551">
+        <v>5</v>
+      </c>
+      <c r="D551">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A552">
+        <v>4</v>
+      </c>
+      <c r="B552">
+        <v>6</v>
+      </c>
+      <c r="C552">
+        <v>6</v>
+      </c>
+      <c r="D552">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A553">
+        <v>1</v>
+      </c>
+      <c r="B553">
+        <v>7</v>
+      </c>
+      <c r="C553">
+        <v>2</v>
+      </c>
+      <c r="D553">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A554">
+        <v>5</v>
+      </c>
+      <c r="B554">
+        <v>13</v>
+      </c>
+      <c r="C554">
+        <v>2</v>
+      </c>
+      <c r="D554">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A555">
+        <v>3</v>
+      </c>
+      <c r="B555">
+        <v>6</v>
+      </c>
+      <c r="C555">
+        <v>4</v>
+      </c>
+      <c r="D555">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A556">
+        <v>5</v>
+      </c>
+      <c r="B556">
+        <v>8</v>
+      </c>
+      <c r="C556">
+        <v>6</v>
+      </c>
+      <c r="D556">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A557">
+        <v>4</v>
+      </c>
+      <c r="B557">
+        <v>2</v>
+      </c>
+      <c r="C557">
+        <v>3</v>
+      </c>
+      <c r="D557">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A558">
+        <v>2</v>
+      </c>
+      <c r="B558">
+        <v>8</v>
+      </c>
+      <c r="C558">
+        <v>5</v>
+      </c>
+      <c r="D558">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A559">
+        <v>5</v>
+      </c>
+      <c r="B559">
+        <v>8</v>
+      </c>
+      <c r="C559">
+        <v>3</v>
+      </c>
+      <c r="D559">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A560">
+        <v>6</v>
+      </c>
+      <c r="B560">
+        <v>14</v>
+      </c>
+      <c r="C560">
+        <v>5</v>
+      </c>
+      <c r="D560">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A561">
+        <v>3</v>
+      </c>
+      <c r="B561">
+        <v>8</v>
+      </c>
+      <c r="C561">
+        <v>2</v>
+      </c>
+      <c r="D561">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A562">
+        <v>7</v>
+      </c>
+      <c r="B562">
+        <v>12</v>
+      </c>
+      <c r="C562">
+        <v>6</v>
+      </c>
+      <c r="D562">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A563">
+        <v>1</v>
+      </c>
+      <c r="B563">
+        <v>8</v>
+      </c>
+      <c r="C563">
+        <v>3</v>
+      </c>
+      <c r="D563">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A564">
+        <v>4</v>
+      </c>
+      <c r="B564">
+        <v>8</v>
+      </c>
+      <c r="C564">
+        <v>2</v>
+      </c>
+      <c r="D564">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="565" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A565">
+        <v>4</v>
+      </c>
+      <c r="B565">
+        <v>6</v>
+      </c>
+      <c r="C565">
+        <v>3</v>
+      </c>
+      <c r="D565">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="566" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A566">
+        <v>5</v>
+      </c>
+      <c r="B566">
+        <v>5</v>
+      </c>
+      <c r="C566">
+        <v>9</v>
+      </c>
+      <c r="D566">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="567" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A567">
+        <v>6</v>
+      </c>
+      <c r="B567">
+        <v>13</v>
+      </c>
+      <c r="C567">
+        <v>4</v>
+      </c>
+      <c r="D567">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="568" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A568">
+        <v>3</v>
+      </c>
+      <c r="B568">
+        <v>13</v>
+      </c>
+      <c r="C568">
+        <v>4</v>
+      </c>
+      <c r="D568">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="569" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A569">
+        <v>2</v>
+      </c>
+      <c r="B569">
+        <v>12</v>
+      </c>
+      <c r="C569">
+        <v>4</v>
+      </c>
+      <c r="D569">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="570" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A570">
+        <v>5</v>
+      </c>
+      <c r="B570">
+        <v>15</v>
+      </c>
+      <c r="C570">
+        <v>4</v>
+      </c>
+      <c r="D570">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="571" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A571">
+        <v>5</v>
+      </c>
+      <c r="B571">
+        <v>6</v>
+      </c>
+      <c r="C571">
+        <v>4</v>
+      </c>
+      <c r="D571">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="572" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A572">
+        <v>5</v>
+      </c>
+      <c r="B572">
+        <v>5</v>
+      </c>
+      <c r="C572">
+        <v>4</v>
+      </c>
+      <c r="D572">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="573" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A573">
+        <v>4</v>
+      </c>
+      <c r="B573">
+        <v>12</v>
+      </c>
+      <c r="C573">
+        <v>5</v>
+      </c>
+      <c r="D573">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="574" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A574">
+        <v>4</v>
+      </c>
+      <c r="B574">
+        <v>4</v>
+      </c>
+      <c r="C574">
+        <v>6</v>
+      </c>
+      <c r="D574">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="575" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A575">
+        <v>5</v>
+      </c>
+      <c r="B575">
+        <v>15</v>
+      </c>
+      <c r="C575">
+        <v>6</v>
+      </c>
+      <c r="D575">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="576" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A576">
+        <v>6</v>
+      </c>
+      <c r="B576">
+        <v>15</v>
+      </c>
+      <c r="C576">
+        <v>4</v>
+      </c>
+      <c r="D576">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="577" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A577">
+        <v>3</v>
+      </c>
+      <c r="B577">
+        <v>5</v>
+      </c>
+      <c r="C577">
+        <v>4</v>
+      </c>
+      <c r="D577">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="578" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A578">
+        <v>2</v>
+      </c>
+      <c r="B578">
+        <v>13</v>
+      </c>
+      <c r="C578">
+        <v>3</v>
+      </c>
+      <c r="D578">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="579" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A579">
+        <v>1</v>
+      </c>
+      <c r="B579">
+        <v>6</v>
+      </c>
+      <c r="C579">
+        <v>2</v>
+      </c>
+      <c r="D579">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="580" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A580">
+        <v>7</v>
+      </c>
+      <c r="B580">
+        <v>8</v>
+      </c>
+      <c r="C580">
+        <v>6</v>
+      </c>
+      <c r="D580">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="581" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A581">
+        <v>4</v>
+      </c>
+      <c r="B581">
+        <v>4</v>
+      </c>
+      <c r="C581">
+        <v>5</v>
+      </c>
+      <c r="D581">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="582" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A582">
+        <v>4</v>
+      </c>
+      <c r="B582">
+        <v>12</v>
+      </c>
+      <c r="C582">
+        <v>2</v>
+      </c>
+      <c r="D582">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="583" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A583">
+        <v>5</v>
+      </c>
+      <c r="B583">
+        <v>12</v>
+      </c>
+      <c r="C583">
+        <v>6</v>
+      </c>
+      <c r="D583">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="584" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A584">
+        <v>3</v>
+      </c>
+      <c r="B584">
+        <v>8</v>
+      </c>
+      <c r="C584">
+        <v>4</v>
+      </c>
+      <c r="D584">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="585" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A585">
+        <v>4</v>
+      </c>
+      <c r="B585">
+        <v>19</v>
+      </c>
+      <c r="C585">
+        <v>3</v>
+      </c>
+      <c r="D585">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="586" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A586">
+        <v>5</v>
+      </c>
+      <c r="B586">
+        <v>16</v>
+      </c>
+      <c r="C586">
+        <v>4</v>
+      </c>
+      <c r="D586">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="587" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A587">
+        <v>5</v>
+      </c>
+      <c r="B587">
+        <v>6</v>
+      </c>
+      <c r="C587">
+        <v>3</v>
+      </c>
+      <c r="D587">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="588" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A588">
+        <v>3</v>
+      </c>
+      <c r="B588">
+        <v>8</v>
+      </c>
+      <c r="C588">
+        <v>4</v>
+      </c>
+      <c r="D588">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="589" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A589">
+        <v>5</v>
+      </c>
+      <c r="B589">
+        <v>15</v>
+      </c>
+      <c r="C589">
+        <v>3</v>
+      </c>
+      <c r="D589">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="590" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A590">
+        <v>2</v>
+      </c>
+      <c r="B590">
+        <v>4</v>
+      </c>
+      <c r="C590">
+        <v>4</v>
+      </c>
+      <c r="D590">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="591" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A591">
+        <v>3</v>
+      </c>
+      <c r="B591">
+        <v>6</v>
+      </c>
+      <c r="C591">
+        <v>2</v>
+      </c>
+      <c r="D591">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="592" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A592">
+        <v>7</v>
+      </c>
+      <c r="B592">
+        <v>5</v>
+      </c>
+      <c r="C592">
+        <v>5</v>
+      </c>
+      <c r="D592">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="593" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A593">
+        <v>4</v>
+      </c>
+      <c r="B593">
+        <v>8</v>
+      </c>
+      <c r="C593">
+        <v>2</v>
+      </c>
+      <c r="D593">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A594">
+        <v>4</v>
+      </c>
+      <c r="B594">
+        <v>8</v>
+      </c>
+      <c r="C594">
+        <v>5</v>
+      </c>
+      <c r="D594">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="595" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A595">
+        <v>4</v>
+      </c>
+      <c r="B595">
+        <v>12</v>
+      </c>
+      <c r="C595">
+        <v>2</v>
+      </c>
+      <c r="D595">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A596">
+        <v>4</v>
+      </c>
+      <c r="B596">
+        <v>8</v>
+      </c>
+      <c r="C596">
+        <v>6</v>
+      </c>
+      <c r="D596">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="597" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A597">
+        <v>6</v>
+      </c>
+      <c r="B597">
+        <v>13</v>
+      </c>
+      <c r="C597">
+        <v>7</v>
+      </c>
+      <c r="D597">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A598">
+        <v>4</v>
+      </c>
+      <c r="B598">
+        <v>15</v>
+      </c>
+      <c r="C598">
+        <v>5</v>
+      </c>
+      <c r="D598">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="599" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A599">
+        <v>4</v>
+      </c>
+      <c r="B599">
+        <v>12</v>
+      </c>
+      <c r="C599">
+        <v>1</v>
+      </c>
+      <c r="D599">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A600">
+        <v>6</v>
+      </c>
+      <c r="B600">
+        <v>16</v>
+      </c>
+      <c r="C600">
+        <v>3</v>
+      </c>
+      <c r="D600">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="601" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A601">
+        <v>4</v>
+      </c>
+      <c r="B601">
+        <v>17</v>
+      </c>
+      <c r="C601">
+        <v>3</v>
+      </c>
+      <c r="D601">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="602" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A602">
+        <v>5</v>
+      </c>
+      <c r="B602">
+        <v>16</v>
+      </c>
+      <c r="C602">
+        <v>4</v>
+      </c>
+      <c r="D602">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="603" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A603">
+        <v>6</v>
+      </c>
+      <c r="B603">
+        <v>12</v>
+      </c>
+      <c r="C603">
+        <v>5</v>
+      </c>
+      <c r="D603">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="604" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A604">
+        <v>2</v>
+      </c>
+      <c r="B604">
+        <v>16</v>
+      </c>
+      <c r="C604">
+        <v>3</v>
+      </c>
+      <c r="D604">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="605" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A605">
+        <v>2</v>
+      </c>
+      <c r="B605">
+        <v>15</v>
+      </c>
+      <c r="C605">
+        <v>3</v>
+      </c>
+      <c r="D605">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="606" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A606">
+        <v>5</v>
+      </c>
+      <c r="B606">
+        <v>7</v>
+      </c>
+      <c r="C606">
+        <v>6</v>
+      </c>
+      <c r="D606">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="607" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A607">
+        <v>6</v>
+      </c>
+      <c r="B607">
+        <v>13</v>
+      </c>
+      <c r="C607">
+        <v>5</v>
+      </c>
+      <c r="D607">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A608">
+        <v>3</v>
+      </c>
+      <c r="B608">
+        <v>12</v>
+      </c>
+      <c r="C608">
+        <v>2</v>
+      </c>
+      <c r="D608">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="609" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A609">
+        <v>3</v>
+      </c>
+      <c r="B609">
+        <v>5</v>
+      </c>
+      <c r="C609">
+        <v>4</v>
+      </c>
+      <c r="D609">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A610">
+        <v>4</v>
+      </c>
+      <c r="B610">
+        <v>7</v>
+      </c>
+      <c r="C610">
+        <v>3</v>
+      </c>
+      <c r="D610">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A611">
+        <v>5</v>
+      </c>
+      <c r="B611">
+        <v>14</v>
+      </c>
+      <c r="C611">
+        <v>8</v>
+      </c>
+      <c r="D611">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="612" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A612">
+        <v>1</v>
+      </c>
+      <c r="B612">
+        <v>8</v>
+      </c>
+      <c r="C612">
+        <v>4</v>
+      </c>
+      <c r="D612">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A613">
+        <v>2</v>
+      </c>
+      <c r="B613">
+        <v>15</v>
+      </c>
+      <c r="C613">
+        <v>3</v>
+      </c>
+      <c r="D613">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="614" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A614">
+        <v>4</v>
+      </c>
+      <c r="B614">
+        <v>13</v>
+      </c>
+      <c r="C614">
+        <v>5</v>
+      </c>
+      <c r="D614">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="615" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A615">
+        <v>2</v>
+      </c>
+      <c r="B615">
+        <v>15</v>
+      </c>
+      <c r="C615">
+        <v>4</v>
+      </c>
+      <c r="D615">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A616">
+        <v>5</v>
+      </c>
+      <c r="B616">
+        <v>12</v>
+      </c>
+      <c r="C616">
+        <v>4</v>
+      </c>
+      <c r="D616">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="617" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A617">
+        <v>6</v>
+      </c>
+      <c r="B617">
+        <v>6</v>
+      </c>
+      <c r="C617">
+        <v>4</v>
+      </c>
+      <c r="D617">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="618" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A618">
+        <v>5</v>
+      </c>
+      <c r="B618">
+        <v>16</v>
+      </c>
+      <c r="C618">
+        <v>4</v>
+      </c>
+      <c r="D618">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="619" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A619">
+        <v>2</v>
+      </c>
+      <c r="B619">
+        <v>6</v>
+      </c>
+      <c r="C619">
+        <v>4</v>
+      </c>
+      <c r="D619">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="620" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A620">
+        <v>1</v>
+      </c>
+      <c r="B620">
+        <v>14</v>
+      </c>
+      <c r="C620">
+        <v>3</v>
+      </c>
+      <c r="D620">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="621" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A621">
+        <v>6</v>
+      </c>
+      <c r="B621">
+        <v>16</v>
+      </c>
+      <c r="C621">
+        <v>4</v>
+      </c>
+      <c r="D621">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="622" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A622">
+        <v>7</v>
+      </c>
+      <c r="B622">
+        <v>5</v>
+      </c>
+      <c r="C622">
+        <v>6</v>
+      </c>
+      <c r="D622">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="623" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A623">
+        <v>6</v>
+      </c>
+      <c r="B623">
+        <v>7</v>
+      </c>
+      <c r="C623">
+        <v>7</v>
+      </c>
+      <c r="D623">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="624" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A624">
+        <v>5</v>
+      </c>
+      <c r="B624">
+        <v>16</v>
+      </c>
+      <c r="C624">
+        <v>4</v>
+      </c>
+      <c r="D624">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A625">
+        <v>5</v>
+      </c>
+      <c r="B625">
+        <v>8</v>
+      </c>
+      <c r="C625">
+        <v>6</v>
+      </c>
+      <c r="D625">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="626" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A626">
+        <v>3</v>
+      </c>
+      <c r="B626">
+        <v>2</v>
+      </c>
+      <c r="C626">
+        <v>4</v>
+      </c>
+      <c r="D626">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="627" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A627">
+        <v>5</v>
+      </c>
+      <c r="B627">
+        <v>7</v>
+      </c>
+      <c r="C627">
+        <v>1</v>
+      </c>
+      <c r="D627">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="628" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A628">
+        <v>5</v>
+      </c>
+      <c r="B628">
+        <v>14</v>
+      </c>
+      <c r="C628">
+        <v>6</v>
+      </c>
+      <c r="D628">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="629" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A629">
+        <v>5</v>
+      </c>
+      <c r="B629">
+        <v>13</v>
+      </c>
+      <c r="C629">
+        <v>6</v>
+      </c>
+      <c r="D629">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="630" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A630">
+        <v>3</v>
+      </c>
+      <c r="B630">
+        <v>5</v>
+      </c>
+      <c r="C630">
+        <v>4</v>
+      </c>
+      <c r="D630">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="631" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A631">
+        <v>5</v>
+      </c>
+      <c r="B631">
+        <v>14</v>
+      </c>
+      <c r="C631">
+        <v>3</v>
+      </c>
+      <c r="D631">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="632" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A632">
+        <v>2</v>
+      </c>
+      <c r="B632">
+        <v>12</v>
+      </c>
+      <c r="C632">
+        <v>3</v>
+      </c>
+      <c r="D632">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="633" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A633">
+        <v>8</v>
+      </c>
+      <c r="B633">
+        <v>17</v>
+      </c>
+      <c r="C633">
+        <v>7</v>
+      </c>
+      <c r="D633">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="634" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A634">
+        <v>1</v>
+      </c>
+      <c r="B634">
+        <v>15</v>
+      </c>
+      <c r="C634">
+        <v>2</v>
+      </c>
+      <c r="D634">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A635">
+        <v>3</v>
+      </c>
+      <c r="B635">
+        <v>1</v>
+      </c>
+      <c r="C635">
+        <v>2</v>
+      </c>
+      <c r="D635">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="636" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A636">
+        <v>4</v>
+      </c>
+      <c r="B636">
+        <v>7</v>
+      </c>
+      <c r="C636">
+        <v>6</v>
+      </c>
+      <c r="D636">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="637" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A637">
+        <v>7</v>
+      </c>
+      <c r="B637">
+        <v>14</v>
+      </c>
+      <c r="C637">
+        <v>6</v>
+      </c>
+      <c r="D637">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="638" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A638">
+        <v>4</v>
+      </c>
+      <c r="B638">
+        <v>14</v>
+      </c>
+      <c r="C638">
+        <v>1</v>
+      </c>
+      <c r="D638">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A639">
+        <v>4</v>
+      </c>
+      <c r="B639">
+        <v>15</v>
+      </c>
+      <c r="C639">
+        <v>2</v>
+      </c>
+      <c r="D639">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="640" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A640">
+        <v>4</v>
+      </c>
+      <c r="B640">
+        <v>18</v>
+      </c>
+      <c r="C640">
+        <v>3</v>
+      </c>
+      <c r="D640">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="641" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A641">
+        <v>5</v>
+      </c>
+      <c r="B641">
+        <v>12</v>
+      </c>
+      <c r="C641">
+        <v>6</v>
+      </c>
+      <c r="D641">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="642" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A642">
+        <v>4</v>
+      </c>
+      <c r="B642">
+        <v>12</v>
+      </c>
+      <c r="C642">
+        <v>5</v>
+      </c>
+      <c r="D642">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="643" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A643">
+        <v>6</v>
+      </c>
+      <c r="B643">
+        <v>4</v>
+      </c>
+      <c r="C643">
+        <v>5</v>
+      </c>
+      <c r="D643">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="644" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A644">
+        <v>5</v>
+      </c>
+      <c r="B644">
+        <v>14</v>
+      </c>
+      <c r="C644">
+        <v>4</v>
+      </c>
+      <c r="D644">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="645" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A645">
+        <v>4</v>
+      </c>
+      <c r="B645">
+        <v>12</v>
+      </c>
+      <c r="C645">
+        <v>3</v>
+      </c>
+      <c r="D645">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="646" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A646">
+        <v>6</v>
+      </c>
+      <c r="B646">
+        <v>17</v>
+      </c>
+      <c r="C646">
+        <v>4</v>
+      </c>
+      <c r="D646">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="647" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A647">
+        <v>5</v>
+      </c>
+      <c r="B647">
+        <v>12</v>
+      </c>
+      <c r="C647">
+        <v>4</v>
+      </c>
+      <c r="D647">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="648" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A648">
+        <v>2</v>
+      </c>
+      <c r="B648">
+        <v>7</v>
+      </c>
+      <c r="C648">
+        <v>3</v>
+      </c>
+      <c r="D648">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="649" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A649">
+        <v>6</v>
+      </c>
+      <c r="B649">
+        <v>5</v>
+      </c>
+      <c r="C649">
+        <v>5</v>
+      </c>
+      <c r="D649">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="650" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A650">
+        <v>2</v>
+      </c>
+      <c r="B650">
+        <v>17</v>
+      </c>
+      <c r="C650">
+        <v>6</v>
+      </c>
+      <c r="D650">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="651" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A651">
+        <v>6</v>
+      </c>
+      <c r="B651">
+        <v>15</v>
+      </c>
+      <c r="C651">
+        <v>5</v>
+      </c>
+      <c r="D651">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A652">
+        <v>3</v>
+      </c>
+      <c r="B652">
+        <v>12</v>
+      </c>
+      <c r="C652">
+        <v>4</v>
+      </c>
+      <c r="D652">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A653">
+        <v>6</v>
+      </c>
+      <c r="B653">
+        <v>13</v>
+      </c>
+      <c r="C653">
+        <v>5</v>
+      </c>
+      <c r="D653">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A654">
+        <v>4</v>
+      </c>
+      <c r="B654">
+        <v>14</v>
+      </c>
+      <c r="C654">
+        <v>2</v>
+      </c>
+      <c r="D654">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A655">
+        <v>1</v>
+      </c>
+      <c r="B655">
+        <v>16</v>
+      </c>
+      <c r="C655">
+        <v>2</v>
+      </c>
+      <c r="D655">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A656">
+        <v>6</v>
+      </c>
+      <c r="B656">
+        <v>7</v>
+      </c>
+      <c r="C656">
+        <v>5</v>
+      </c>
+      <c r="D656">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A657">
+        <v>4</v>
+      </c>
+      <c r="B657">
+        <v>7</v>
+      </c>
+      <c r="C657">
+        <v>9</v>
+      </c>
+      <c r="D657">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="658" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A658">
+        <v>7</v>
+      </c>
+      <c r="B658">
+        <v>15</v>
+      </c>
+      <c r="C658">
+        <v>4</v>
+      </c>
+      <c r="D658">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="659" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A659">
+        <v>2</v>
+      </c>
+      <c r="B659">
+        <v>13</v>
+      </c>
+      <c r="C659">
+        <v>4</v>
+      </c>
+      <c r="D659">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A660">
+        <v>5</v>
+      </c>
+      <c r="B660">
+        <v>6</v>
+      </c>
+      <c r="C660">
+        <v>4</v>
+      </c>
+      <c r="D660">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A661">
+        <v>6</v>
+      </c>
+      <c r="B661">
+        <v>16</v>
+      </c>
+      <c r="C661">
+        <v>7</v>
+      </c>
+      <c r="D661">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="662" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A662">
+        <v>3</v>
+      </c>
+      <c r="B662">
+        <v>6</v>
+      </c>
+      <c r="C662">
+        <v>4</v>
+      </c>
+      <c r="D662">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="663" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A663">
+        <v>5</v>
+      </c>
+      <c r="B663">
+        <v>6</v>
+      </c>
+      <c r="C663">
+        <v>3</v>
+      </c>
+      <c r="D663">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="664" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A664">
+        <v>6</v>
+      </c>
+      <c r="B664">
+        <v>8</v>
+      </c>
+      <c r="C664">
+        <v>4</v>
+      </c>
+      <c r="D664">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="665" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A665">
+        <v>5</v>
+      </c>
+      <c r="B665">
+        <v>5</v>
+      </c>
+      <c r="C665">
+        <v>4</v>
+      </c>
+      <c r="D665">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="666" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A666">
+        <v>4</v>
+      </c>
+      <c r="B666">
+        <v>2</v>
+      </c>
+      <c r="C666">
+        <v>5</v>
+      </c>
+      <c r="D666">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="667" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A667">
+        <v>4</v>
+      </c>
+      <c r="B667">
+        <v>8</v>
+      </c>
+      <c r="C667">
+        <v>7</v>
+      </c>
+      <c r="D667">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="668" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A668">
+        <v>5</v>
+      </c>
+      <c r="B668">
+        <v>6</v>
+      </c>
+      <c r="C668">
+        <v>6</v>
+      </c>
+      <c r="D668">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A669">
+        <v>2</v>
+      </c>
+      <c r="B669">
+        <v>8</v>
+      </c>
+      <c r="C669">
+        <v>1</v>
+      </c>
+      <c r="D669">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="670" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A670">
+        <v>3</v>
+      </c>
+      <c r="B670">
+        <v>17</v>
+      </c>
+      <c r="C670">
+        <v>4</v>
+      </c>
+      <c r="D670">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="671" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A671">
+        <v>5</v>
+      </c>
+      <c r="B671">
+        <v>5</v>
+      </c>
+      <c r="C671">
+        <v>6</v>
+      </c>
+      <c r="D671">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="672" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A672">
+        <v>4</v>
+      </c>
+      <c r="B672">
+        <v>12</v>
+      </c>
+      <c r="C672">
+        <v>2</v>
+      </c>
+      <c r="D672">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="673" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A673">
+        <v>5</v>
+      </c>
+      <c r="B673">
+        <v>7</v>
+      </c>
+      <c r="C673">
+        <v>6</v>
+      </c>
+      <c r="D673">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="674" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A674">
+        <v>3</v>
+      </c>
+      <c r="B674">
+        <v>12</v>
+      </c>
+      <c r="C674">
+        <v>5</v>
+      </c>
+      <c r="D674">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="675" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A675">
+        <v>3</v>
+      </c>
+      <c r="B675">
+        <v>14</v>
+      </c>
+      <c r="C675">
+        <v>6</v>
+      </c>
+      <c r="D675">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="676" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A676">
+        <v>5</v>
+      </c>
+      <c r="B676">
+        <v>7</v>
+      </c>
+      <c r="C676">
+        <v>6</v>
+      </c>
+      <c r="D676">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="677" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A677">
+        <v>6</v>
+      </c>
+      <c r="B677">
+        <v>12</v>
+      </c>
+      <c r="C677">
+        <v>3</v>
+      </c>
+      <c r="D677">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="678" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A678">
+        <v>3</v>
+      </c>
+      <c r="B678">
+        <v>8</v>
+      </c>
+      <c r="C678">
+        <v>4</v>
+      </c>
+      <c r="D678">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="679" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A679">
+        <v>5</v>
+      </c>
+      <c r="B679">
+        <v>13</v>
+      </c>
+      <c r="C679">
+        <v>4</v>
+      </c>
+      <c r="D679">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>